<commit_message>
Auto stash before merge of "master" and "origin/master"
</commit_message>
<xml_diff>
--- a/Gestion de Projet/Objectifs - Projet Supervision.xlsx
+++ b/Gestion de Projet/Objectifs - Projet Supervision.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="28800" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -567,6 +567,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -613,12 +619,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -961,7 +961,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1008,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="27" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -1025,13 +1025,13 @@
         <f>IF(A10&gt;=9,"A",IF(A10&gt;=7,"B",IF(A10&gt;=4,"C","D")))</f>
         <v>A</v>
       </c>
-      <c r="F5" s="41">
+      <c r="F5" s="25">
         <f>IF(E5="A",5,IF(E5="B",4,IF(E5="C",2,IF(E5="D",1,0))))</f>
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="26"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1043,10 +1043,10 @@
         <v>1</v>
       </c>
       <c r="E6" s="60"/>
-      <c r="F6" s="41"/>
+      <c r="F6" s="25"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
@@ -1058,10 +1058,10 @@
         <v>0</v>
       </c>
       <c r="E7" s="60"/>
-      <c r="F7" s="41"/>
+      <c r="F7" s="25"/>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
@@ -1073,33 +1073,33 @@
         <v>1</v>
       </c>
       <c r="E8" s="60"/>
-      <c r="F8" s="41"/>
+      <c r="F8" s="25"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="24">
         <f>D9*2</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E9" s="60"/>
-      <c r="F9" s="41"/>
+      <c r="F9" s="25"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="57">
         <f>SUM(C5:C9)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="58"/>
       <c r="C10" s="58"/>
       <c r="D10" s="58"/>
       <c r="E10" s="61"/>
-      <c r="F10" s="41"/>
+      <c r="F10" s="25"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="49" t="s">
@@ -1115,11 +1115,11 @@
       <c r="D11" s="10">
         <v>1</v>
       </c>
-      <c r="E11" s="27" t="str">
+      <c r="E11" s="29" t="str">
         <f>IF(A14&gt;=6,"A",IF(A14&gt;=4,"B",IF(A14&gt;=2,"C","D")))</f>
         <v>A</v>
       </c>
-      <c r="F11" s="41">
+      <c r="F11" s="25">
         <f>IF(E11="A",5,IF(E11="B",4,IF(E11="C",2,IF(E11="D",1,0))))</f>
         <v>5</v>
       </c>
@@ -1136,8 +1136,8 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="F12" s="41"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="25"/>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="50"/>
@@ -1151,8 +1151,8 @@
       <c r="D13" s="1">
         <v>1</v>
       </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="41"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="25"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="51">
@@ -1162,8 +1162,8 @@
       <c r="B14" s="52"/>
       <c r="C14" s="52"/>
       <c r="D14" s="52"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="41"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="25"/>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="53" t="s">
@@ -1174,18 +1174,18 @@
       </c>
       <c r="C15" s="18">
         <f>D15*3</f>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="D15" s="10">
-        <v>0.5</v>
-      </c>
-      <c r="E15" s="30" t="str">
+        <v>1</v>
+      </c>
+      <c r="E15" s="32" t="str">
         <f>IF(A20&gt;=9,"A",IF(A20&gt;=7,"B",IF(A20&gt;=4,"C","D")))</f>
-        <v>C</v>
-      </c>
-      <c r="F15" s="41">
+        <v>A</v>
+      </c>
+      <c r="F15" s="25">
         <f>IF(E15="A",5,IF(E15="B",4,IF(E15="C",2,IF(E15="D",1,0))))</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1200,8 +1200,8 @@
       <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="41"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="25"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="54"/>
@@ -1215,8 +1215,8 @@
       <c r="D17" s="1">
         <v>1</v>
       </c>
-      <c r="E17" s="31"/>
-      <c r="F17" s="41"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="25"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="54"/>
@@ -1225,13 +1225,13 @@
       </c>
       <c r="C18" s="19">
         <f>D18*2</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18" s="1">
-        <v>0</v>
-      </c>
-      <c r="E18" s="31"/>
-      <c r="F18" s="41"/>
+        <v>1</v>
+      </c>
+      <c r="E18" s="33"/>
+      <c r="F18" s="25"/>
     </row>
     <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="54"/>
@@ -1240,24 +1240,24 @@
       </c>
       <c r="C19" s="20">
         <f>D19*1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>0</v>
-      </c>
-      <c r="E19" s="31"/>
-      <c r="F19" s="41"/>
+        <v>1</v>
+      </c>
+      <c r="E19" s="33"/>
+      <c r="F19" s="25"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="55">
         <f>SUM(C15:C19)</f>
-        <v>6.5</v>
+        <v>11</v>
       </c>
       <c r="B20" s="56"/>
       <c r="C20" s="56"/>
       <c r="D20" s="56"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="41"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="25"/>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="43" t="s">
@@ -1275,11 +1275,11 @@
       </c>
       <c r="E21" s="45" t="str">
         <f>IF(A24=3,"A",IF(A24=2,"B",IF(A24=1,"C","D")))</f>
-        <v>A</v>
-      </c>
-      <c r="F21" s="41">
+        <v>B</v>
+      </c>
+      <c r="F21" s="25">
         <f>IF(E21="A",5,IF(E21="B",4,IF(E21="C",2,IF(E21="D",1,0))))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1289,13 +1289,13 @@
       </c>
       <c r="C22" s="17">
         <f>D22*1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="46"/>
-      <c r="F22" s="41"/>
+      <c r="F22" s="25"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="44"/>
@@ -1310,50 +1310,45 @@
         <v>1</v>
       </c>
       <c r="E23" s="46"/>
-      <c r="F23" s="41"/>
+      <c r="F23" s="25"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="47">
         <f>SUM(C21:C23)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B24" s="48"/>
       <c r="C24" s="48"/>
       <c r="D24" s="48"/>
       <c r="E24" s="46"/>
-      <c r="F24" s="41"/>
+      <c r="F24" s="25"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="39" t="str">
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="41" t="str">
         <f>IF(F25&gt;=4.6,"A",IF(F25&gt;=3.6,"B",IF(F25&gt;=2.6,"C","D")))</f>
-        <v>B</v>
-      </c>
-      <c r="F25" s="42">
+        <v>A</v>
+      </c>
+      <c r="F25" s="26">
         <f>SUM(F5:F24)/4</f>
-        <v>4.25</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="36"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="38"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="42"/>
+      <c r="A26" s="38"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="F5:F10"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="F15:F20"/>
-    <mergeCell ref="F21:F24"/>
-    <mergeCell ref="F25:F26"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="E15:E20"/>
@@ -1368,6 +1363,11 @@
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="E5:E10"/>
+    <mergeCell ref="F5:F10"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="F15:F20"/>
+    <mergeCell ref="F21:F24"/>
+    <mergeCell ref="F25:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Ajout du Suivi du Projet
</commit_message>
<xml_diff>
--- a/Gestion de Projet/Objectifs - Projet Supervision.xlsx
+++ b/Gestion de Projet/Objectifs - Projet Supervision.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="900" windowWidth="28800" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1350" windowWidth="28800" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -567,116 +567,116 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -961,7 +961,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1008,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="25" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -1021,17 +1021,17 @@
       <c r="D5" s="10">
         <v>1</v>
       </c>
-      <c r="E5" s="59" t="str">
+      <c r="E5" s="57" t="str">
         <f>IF(A10&gt;=9,"A",IF(A10&gt;=7,"B",IF(A10&gt;=4,"C","D")))</f>
         <v>A</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="60">
         <f>IF(E5="A",5,IF(E5="B",4,IF(E5="C",2,IF(E5="D",1,0))))</f>
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -1042,11 +1042,11 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="60"/>
-      <c r="F6" s="25"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="60"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
@@ -1057,11 +1057,11 @@
       <c r="D7" s="1">
         <v>0</v>
       </c>
-      <c r="E7" s="60"/>
-      <c r="F7" s="25"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="60"/>
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
@@ -1072,11 +1072,11 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="60"/>
-      <c r="F8" s="25"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="60"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
@@ -1087,22 +1087,22 @@
       <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="60"/>
-      <c r="F9" s="25"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="60"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="57">
+      <c r="A10" s="55">
         <f>SUM(C5:C9)</f>
         <v>10</v>
       </c>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="25"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="60"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="47" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -1115,17 +1115,17 @@
       <c r="D11" s="10">
         <v>1</v>
       </c>
-      <c r="E11" s="29" t="str">
+      <c r="E11" s="27" t="str">
         <f>IF(A14&gt;=6,"A",IF(A14&gt;=4,"B",IF(A14&gt;=2,"C","D")))</f>
         <v>A</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="60">
         <f>IF(E11="A",5,IF(E11="B",4,IF(E11="C",2,IF(E11="D",1,0))))</f>
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="50"/>
+      <c r="A12" s="48"/>
       <c r="B12" s="6" t="s">
         <v>23</v>
       </c>
@@ -1136,11 +1136,11 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="25"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="60"/>
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
+      <c r="A13" s="48"/>
       <c r="B13" s="6" t="s">
         <v>8</v>
       </c>
@@ -1151,22 +1151,22 @@
       <c r="D13" s="1">
         <v>1</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="25"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="60"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="51">
+      <c r="A14" s="49">
         <f>SUM(C11:C13)</f>
         <v>7</v>
       </c>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="25"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="60"/>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="53" t="s">
+      <c r="A15" s="51" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -1179,17 +1179,17 @@
       <c r="D15" s="10">
         <v>1</v>
       </c>
-      <c r="E15" s="32" t="str">
+      <c r="E15" s="30" t="str">
         <f>IF(A20&gt;=9,"A",IF(A20&gt;=7,"B",IF(A20&gt;=4,"C","D")))</f>
         <v>A</v>
       </c>
-      <c r="F15" s="25">
+      <c r="F15" s="60">
         <f>IF(E15="A",5,IF(E15="B",4,IF(E15="C",2,IF(E15="D",1,0))))</f>
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="54"/>
+      <c r="A16" s="52"/>
       <c r="B16" s="6" t="s">
         <v>11</v>
       </c>
@@ -1200,11 +1200,11 @@
       <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="25"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="60"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
+      <c r="A17" s="52"/>
       <c r="B17" s="6" t="s">
         <v>16</v>
       </c>
@@ -1215,11 +1215,11 @@
       <c r="D17" s="1">
         <v>1</v>
       </c>
-      <c r="E17" s="33"/>
-      <c r="F17" s="25"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="60"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="54"/>
+      <c r="A18" s="52"/>
       <c r="B18" s="6" t="s">
         <v>12</v>
       </c>
@@ -1230,11 +1230,11 @@
       <c r="D18" s="1">
         <v>1</v>
       </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="25"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="60"/>
     </row>
     <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="54"/>
+      <c r="A19" s="52"/>
       <c r="B19" s="2" t="s">
         <v>15</v>
       </c>
@@ -1245,22 +1245,22 @@
       <c r="D19" s="1">
         <v>1</v>
       </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="25"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="60"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="55">
+      <c r="A20" s="53">
         <f>SUM(C15:C19)</f>
         <v>11</v>
       </c>
-      <c r="B20" s="56"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="25"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="60"/>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="43" t="s">
+      <c r="A21" s="41" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="12" t="s">
@@ -1273,32 +1273,32 @@
       <c r="D21" s="13">
         <v>1</v>
       </c>
-      <c r="E21" s="45" t="str">
+      <c r="E21" s="43" t="str">
         <f>IF(A24=3,"A",IF(A24=2,"B",IF(A24=1,"C","D")))</f>
-        <v>B</v>
-      </c>
-      <c r="F21" s="25">
+        <v>A</v>
+      </c>
+      <c r="F21" s="60">
         <f>IF(E21="A",5,IF(E21="B",4,IF(E21="C",2,IF(E21="D",1,0))))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
+      <c r="A22" s="42"/>
       <c r="B22" s="2" t="s">
         <v>24</v>
       </c>
       <c r="C22" s="17">
         <f>D22*1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="1">
-        <v>0</v>
-      </c>
-      <c r="E22" s="46"/>
-      <c r="F22" s="25"/>
+        <v>1</v>
+      </c>
+      <c r="E22" s="44"/>
+      <c r="F22" s="60"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
+      <c r="A23" s="42"/>
       <c r="B23" s="2" t="s">
         <v>14</v>
       </c>
@@ -1309,46 +1309,51 @@
       <c r="D23" s="1">
         <v>1</v>
       </c>
-      <c r="E23" s="46"/>
-      <c r="F23" s="25"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="60"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="47">
+      <c r="A24" s="45">
         <f>SUM(C21:C23)</f>
-        <v>2</v>
-      </c>
-      <c r="B24" s="48"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="25"/>
+        <v>3</v>
+      </c>
+      <c r="B24" s="46"/>
+      <c r="C24" s="46"/>
+      <c r="D24" s="46"/>
+      <c r="E24" s="44"/>
+      <c r="F24" s="60"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
+      <c r="A25" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="41" t="str">
+      <c r="B25" s="34"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="39" t="str">
         <f>IF(F25&gt;=4.6,"A",IF(F25&gt;=3.6,"B",IF(F25&gt;=2.6,"C","D")))</f>
         <v>A</v>
       </c>
-      <c r="F25" s="26">
+      <c r="F25" s="61">
         <f>SUM(F5:F24)/4</f>
-        <v>4.75</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="38"/>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="26"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="F5:F10"/>
+    <mergeCell ref="F11:F14"/>
+    <mergeCell ref="F15:F20"/>
+    <mergeCell ref="F21:F24"/>
+    <mergeCell ref="F25:F26"/>
     <mergeCell ref="A5:A9"/>
     <mergeCell ref="E11:E14"/>
     <mergeCell ref="E15:E20"/>
@@ -1363,11 +1368,6 @@
     <mergeCell ref="A20:D20"/>
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="E5:E10"/>
-    <mergeCell ref="F5:F10"/>
-    <mergeCell ref="F11:F14"/>
-    <mergeCell ref="F15:F20"/>
-    <mergeCell ref="F21:F24"/>
-    <mergeCell ref="F25:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>